<commit_message>
Updated Pretty.hs, started TypeCheck.hs
Added updated journal log, time/labor. Tenatively finished Pretty.hs (testing tomorrow), started TypeCheck.hs.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-23may2016 .xlsx
+++ b/time-labor/week-of-23may2016 .xlsx
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -587,17 +588,17 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.35204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.21428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -823,16 +824,16 @@
         <v>24</v>
       </c>
       <c r="C14" s="19" t="n">
-        <v>0</v>
+        <v>0.4375</v>
       </c>
       <c r="D14" s="20" t="n">
-        <v>0</v>
+        <v>0.645833333333333</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="21" t="n">
         <f aca="false">IF((((D14-C14)+(F14-E14))*24)&gt;8,8,((D14-C14)+(F14-E14))*24)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H14" s="21" t="n">
         <f aca="false">IF(((D14-C14)+(F14-E14))*24&gt;8,((D14-C14)+(F14-E14))*24-8,0)</f>
@@ -847,16 +848,16 @@
         <v>25</v>
       </c>
       <c r="C15" s="19" t="n">
-        <v>0</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D15" s="20" t="n">
-        <v>0</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="21" t="n">
         <f aca="false">IF((((D15-C15)+(F15-E15))*24)&gt;8,8,((D15-C15)+(F15-E15))*24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="21" t="n">
         <f aca="false">IF(((D15-C15)+(F15-E15))*24&gt;8,((D15-C15)+(F15-E15))*24-8,0)</f>
@@ -871,16 +872,16 @@
         <v>26</v>
       </c>
       <c r="C16" s="19" t="n">
-        <v>0</v>
+        <v>0.520833333333333</v>
       </c>
       <c r="D16" s="20" t="n">
-        <v>0</v>
+        <v>0.729166666666667</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21" t="n">
         <f aca="false">IF((((D16-C16)+(F16-E16))*24)&gt;8,8,((D16-C16)+(F16-E16))*24)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H16" s="21" t="n">
         <f aca="false">IF(((D16-C16)+(F16-E16))*24&gt;8,((D16-C16)+(F16-E16))*24-8,0)</f>
@@ -972,7 +973,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1016,7 +1017,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1032,7 +1033,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>50</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>